<commit_message>
feat: apply median filter to model predictions
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="64">
   <si>
     <t>Seizures</t>
   </si>
@@ -134,9 +134,6 @@
     <t>RandomUnderSampler(sampling_strategy</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>0.8</t>
   </si>
   <si>
@@ -177,6 +174,48 @@
   </si>
   <si>
     <t>0.52</t>
+  </si>
+  <si>
+    <t>Post-Processing (The "Logic" Fix)</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>0.67</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>Yes (5)</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>0.62</t>
+  </si>
+  <si>
+    <t>0.77</t>
+  </si>
+  <si>
+    <t>0.025</t>
+  </si>
+  <si>
+    <t>0.78</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.88</t>
   </si>
 </sst>
 </file>
@@ -495,370 +534,406 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" customWidth="1"/>
-    <col min="5" max="5" width="30.5546875" customWidth="1"/>
+    <col min="2" max="3" width="27.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.44140625" customWidth="1"/>
+    <col min="5" max="5" width="35.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2">
         <v>387489</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>129163</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3">
         <v>129162</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>43054</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4">
         <v>312141</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>43054</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>29</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5">
         <v>215270</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>43054</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>26</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6">
         <v>150689</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>43054</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>23</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>114810</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>43054</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>19</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>20</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8">
         <v>96871</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>43054</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>17</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9">
         <v>86108</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>43054</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>14</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>15</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10">
         <v>172218</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>86109</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>6</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>12</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
         <v>44</v>
       </c>
-      <c r="D11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11">
+      <c r="F11">
         <v>129162</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>64581</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>9</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>10</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12">
         <v>258326</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>129163</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>6</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>7</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -866,112 +941,284 @@
         <v>47</v>
       </c>
       <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
         <v>41</v>
       </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13">
-        <v>430546</v>
+      <c r="E13" t="s">
+        <v>44</v>
       </c>
       <c r="F13">
-        <v>215273</v>
-      </c>
-      <c r="G13" t="s">
-        <v>36</v>
+        <v>86108</v>
+      </c>
+      <c r="G13">
+        <v>43054</v>
       </c>
       <c r="H13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="J13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14">
+        <v>96871</v>
+      </c>
+      <c r="G14">
+        <v>43054</v>
+      </c>
+      <c r="H14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" t="s">
         <v>48</v>
       </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14">
-        <v>86108</v>
-      </c>
-      <c r="F14">
-        <v>43054</v>
-      </c>
-      <c r="G14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
         <v>42</v>
       </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15">
-        <v>96871</v>
+      <c r="E15" t="s">
+        <v>44</v>
       </c>
       <c r="F15">
-        <v>43054</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
+        <v>172218</v>
+      </c>
+      <c r="G15">
+        <v>86109</v>
       </c>
       <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" t="s">
         <v>49</v>
       </c>
-      <c r="I15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16">
         <v>172218</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>86109</v>
       </c>
-      <c r="G16" t="s">
-        <v>6</v>
-      </c>
       <c r="H16" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="I16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17">
+        <v>301380</v>
+      </c>
+      <c r="G17">
+        <v>129163</v>
+      </c>
+      <c r="H17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18">
+        <v>86108</v>
+      </c>
+      <c r="G18">
+        <v>43054</v>
+      </c>
+      <c r="H18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19">
+        <v>43054</v>
+      </c>
+      <c r="G19">
+        <v>21527</v>
+      </c>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20">
+        <v>21526</v>
+      </c>
+      <c r="G20">
+        <v>10763</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21">
+        <v>8610</v>
+      </c>
+      <c r="G21">
+        <v>4305</v>
+      </c>
+      <c r="H21" t="s">
         <v>21</v>
+      </c>
+      <c r="I21" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>